<commit_message>
Load number of stages, jobs and machines from file
</commit_message>
<xml_diff>
--- a/FlowShopInputData.xlsx
+++ b/FlowShopInputData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\C#\FindMinCMax\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7380" tabRatio="712" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7380" tabRatio="712"/>
   </bookViews>
   <sheets>
     <sheet name="Stages and Jobs" sheetId="1" r:id="rId1"/>
@@ -255,9 +255,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -267,16 +264,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,20 +604,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="27"/>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="26">
-        <v>3</v>
+      <c r="A2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="23">
+        <v>300</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -627,8 +627,8 @@
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18">
-        <v>5</v>
+      <c r="B3" s="17">
+        <v>500</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
@@ -657,14 +657,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="25"/>
+      <c r="A1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -672,10 +672,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="17">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -683,18 +683,18 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="23">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>1</v>
       </c>
     </row>
@@ -722,12 +722,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -736,16 +736,16 @@
       <c r="B2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="29"/>
       <c r="J2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="6">
@@ -762,7 +762,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -777,7 +777,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="8">
         <v>3</v>
       </c>
@@ -785,7 +785,7 @@
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="8">
         <v>4</v>
       </c>
@@ -807,7 +807,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="14">
         <v>2</v>
       </c>
       <c r="B8" s="6">
@@ -816,10 +816,10 @@
       <c r="C8" s="7">
         <v>2</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="8">
         <v>2</v>
       </c>
@@ -831,7 +831,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="8">
         <v>3</v>
       </c>
@@ -841,7 +841,7 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="8">
         <v>4</v>
       </c>
@@ -861,7 +861,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="A13" s="14">
         <v>3</v>
       </c>
       <c r="B13" s="6">
@@ -870,10 +870,10 @@
       <c r="C13" s="7">
         <v>1</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="8">
         <v>2</v>
       </c>
@@ -881,7 +881,7 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="8">
         <v>3</v>
       </c>
@@ -891,7 +891,7 @@
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="8">
         <v>4</v>
       </c>
@@ -908,7 +908,7 @@
       <c r="C17" s="11">
         <v>1</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -935,24 +935,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -960,7 +960,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="7">
@@ -969,7 +969,7 @@
       <c r="C3" s="6">
         <v>1</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -977,7 +977,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="9"/>
       <c r="C4" s="8">
         <v>2</v>
@@ -987,7 +987,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="9"/>
       <c r="C5" s="8">
         <v>3</v>
@@ -997,7 +997,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="9"/>
       <c r="C6" s="8">
         <v>4</v>
@@ -1007,17 +1007,17 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="11"/>
       <c r="C7" s="10">
         <v>5</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="9">
         <v>2</v>
       </c>
@@ -1029,32 +1029,32 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="9"/>
       <c r="C9" s="8">
         <v>2</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="9"/>
       <c r="C10" s="8">
         <v>3</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="9"/>
       <c r="C11" s="8">
         <v>4</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <v>10</v>
       </c>
     </row>
@@ -1064,7 +1064,7 @@
       <c r="C12" s="10">
         <v>5</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>14</v>
       </c>
     </row>
@@ -1078,7 +1078,7 @@
       <c r="C13" s="5">
         <v>1</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1088,7 +1088,7 @@
       <c r="C14" s="5">
         <v>2</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="20">
         <v>11</v>
       </c>
     </row>
@@ -1098,7 +1098,7 @@
       <c r="C15" s="5">
         <v>3</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="20">
         <v>9</v>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       <c r="C16" s="5">
         <v>4</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1118,7 +1118,7 @@
       <c r="C17" s="10">
         <v>5</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="17">
         <v>6</v>
       </c>
     </row>
@@ -1130,7 +1130,7 @@
       <c r="C18" s="5">
         <v>1</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="20">
         <v>8</v>
       </c>
     </row>
@@ -1140,7 +1140,7 @@
       <c r="C19" s="5">
         <v>2</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="20">
         <v>4</v>
       </c>
     </row>
@@ -1150,7 +1150,7 @@
       <c r="C20" s="5">
         <v>3</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       <c r="C21" s="5">
         <v>4</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1170,7 +1170,7 @@
       <c r="C22" s="10">
         <v>5</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="17">
         <v>12</v>
       </c>
     </row>
@@ -1184,7 +1184,7 @@
       <c r="C23" s="5">
         <v>1</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="20">
         <v>6</v>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       <c r="C24" s="5">
         <v>2</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1204,7 +1204,7 @@
       <c r="C25" s="5">
         <v>3</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="20">
         <v>8</v>
       </c>
     </row>
@@ -1214,7 +1214,7 @@
       <c r="C26" s="5">
         <v>4</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="20">
         <v>6</v>
       </c>
     </row>
@@ -1224,7 +1224,7 @@
       <c r="C27" s="10">
         <v>5</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="17">
         <v>3</v>
       </c>
     </row>
@@ -1251,24 +1251,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1276,7 +1276,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="7">
@@ -1285,7 +1285,7 @@
       <c r="C3" s="6">
         <v>1</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1293,7 +1293,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="9"/>
       <c r="C4" s="8">
         <v>2</v>
@@ -1303,7 +1303,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="9"/>
       <c r="C5" s="8">
         <v>3</v>
@@ -1313,7 +1313,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="9"/>
       <c r="C6" s="8">
         <v>4</v>
@@ -1323,17 +1323,17 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="11"/>
       <c r="C7" s="10">
         <v>5</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>-5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="9">
         <v>2</v>
       </c>
@@ -1345,32 +1345,32 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="9"/>
       <c r="C9" s="8">
         <v>2</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <v>-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="9"/>
       <c r="C10" s="8">
         <v>3</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="9"/>
       <c r="C11" s="8">
         <v>4</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <v>1</v>
       </c>
     </row>
@@ -1380,7 +1380,7 @@
       <c r="C12" s="10">
         <v>5</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>-6</v>
       </c>
     </row>
@@ -1394,7 +1394,7 @@
       <c r="C13" s="5">
         <v>1</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1404,7 +1404,7 @@
       <c r="C14" s="5">
         <v>2</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1414,7 +1414,7 @@
       <c r="C15" s="5">
         <v>3</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="20">
         <v>3</v>
       </c>
     </row>
@@ -1424,7 +1424,7 @@
       <c r="C16" s="5">
         <v>4</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1434,7 +1434,7 @@
       <c r="C17" s="10">
         <v>5</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="17">
         <v>-3</v>
       </c>
     </row>
@@ -1446,7 +1446,7 @@
       <c r="C18" s="5">
         <v>1</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="20">
         <v>-4</v>
       </c>
     </row>
@@ -1456,7 +1456,7 @@
       <c r="C19" s="5">
         <v>2</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
       <c r="C20" s="5">
         <v>3</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1476,7 +1476,7 @@
       <c r="C21" s="5">
         <v>4</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1486,7 +1486,7 @@
       <c r="C22" s="10">
         <v>5</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="17">
         <v>8</v>
       </c>
     </row>
@@ -1502,9 +1502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J125" sqref="J125"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,28 +1514,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1552,7 +1552,7 @@
       <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="22">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1563,7 +1563,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="3"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="19">
+      <c r="D4" s="18">
         <v>2</v>
       </c>
       <c r="E4">
@@ -1574,7 +1574,7 @@
       <c r="A5" s="4"/>
       <c r="B5" s="3"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="19">
+      <c r="D5" s="18">
         <v>3</v>
       </c>
     </row>
@@ -1582,7 +1582,7 @@
       <c r="A6" s="4"/>
       <c r="B6" s="3"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="19">
+      <c r="D6" s="18">
         <v>4</v>
       </c>
     </row>
@@ -1590,10 +1590,10 @@
       <c r="A7" s="4"/>
       <c r="B7" s="3"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="22">
-        <v>5</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="D7" s="21">
+        <v>5</v>
+      </c>
+      <c r="E7" s="17">
         <v>4</v>
       </c>
     </row>
@@ -1603,7 +1603,7 @@
       <c r="C8" s="5">
         <v>2</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="22">
         <v>1</v>
       </c>
       <c r="E8">
@@ -1614,7 +1614,7 @@
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="19">
+      <c r="D9" s="18">
         <v>2</v>
       </c>
     </row>
@@ -1622,7 +1622,7 @@
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <v>3</v>
       </c>
     </row>
@@ -1630,7 +1630,7 @@
       <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>4</v>
       </c>
     </row>
@@ -1638,10 +1638,10 @@
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="22">
-        <v>5</v>
-      </c>
-      <c r="E12" s="18">
+      <c r="D12" s="21">
+        <v>5</v>
+      </c>
+      <c r="E12" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1651,7 +1651,7 @@
       <c r="C13" s="5">
         <v>3</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1659,7 +1659,7 @@
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="19">
+      <c r="D14" s="18">
         <v>2</v>
       </c>
     </row>
@@ -1667,7 +1667,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="19">
+      <c r="D15" s="18">
         <v>3</v>
       </c>
     </row>
@@ -1675,7 +1675,7 @@
       <c r="A16" s="4"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="19">
+      <c r="D16" s="18">
         <v>4</v>
       </c>
     </row>
@@ -1683,10 +1683,10 @@
       <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="C17" s="10"/>
-      <c r="D17" s="22">
-        <v>5</v>
-      </c>
-      <c r="E17" s="18"/>
+      <c r="D17" s="21">
+        <v>5</v>
+      </c>
+      <c r="E17" s="17"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
@@ -1694,7 +1694,7 @@
       <c r="C18" s="5">
         <v>4</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1702,7 +1702,7 @@
       <c r="A19" s="4"/>
       <c r="B19" s="3"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="19">
+      <c r="D19" s="18">
         <v>2</v>
       </c>
     </row>
@@ -1710,7 +1710,7 @@
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="19">
+      <c r="D20" s="18">
         <v>3</v>
       </c>
     </row>
@@ -1718,7 +1718,7 @@
       <c r="A21" s="4"/>
       <c r="B21" s="3"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="19">
+      <c r="D21" s="18">
         <v>4</v>
       </c>
     </row>
@@ -1726,10 +1726,10 @@
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="22">
-        <v>5</v>
-      </c>
-      <c r="E22" s="18"/>
+      <c r="D22" s="21">
+        <v>5</v>
+      </c>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
@@ -1737,7 +1737,7 @@
       <c r="C23" s="5">
         <v>5</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="22">
         <v>1</v>
       </c>
       <c r="E23">
@@ -1748,7 +1748,7 @@
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="19">
+      <c r="D24" s="18">
         <v>2</v>
       </c>
     </row>
@@ -1756,7 +1756,7 @@
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="19">
+      <c r="D25" s="18">
         <v>3</v>
       </c>
     </row>
@@ -1764,7 +1764,7 @@
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="19">
+      <c r="D26" s="18">
         <v>4</v>
       </c>
     </row>
@@ -1772,10 +1772,10 @@
       <c r="A27" s="4"/>
       <c r="B27" s="11"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="22">
-        <v>5</v>
-      </c>
-      <c r="E27" s="18"/>
+      <c r="D27" s="21">
+        <v>5</v>
+      </c>
+      <c r="E27" s="17"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
@@ -1785,7 +1785,7 @@
       <c r="C28" s="5">
         <v>1</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="19">
+      <c r="D29" s="18">
         <v>2</v>
       </c>
       <c r="E29">
@@ -1804,7 +1804,7 @@
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="19">
+      <c r="D30" s="18">
         <v>3</v>
       </c>
     </row>
@@ -1812,7 +1812,7 @@
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="5"/>
-      <c r="D31" s="19">
+      <c r="D31" s="18">
         <v>4</v>
       </c>
       <c r="E31">
@@ -1823,10 +1823,10 @@
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="10"/>
-      <c r="D32" s="22">
-        <v>5</v>
-      </c>
-      <c r="E32" s="18">
+      <c r="D32" s="21">
+        <v>5</v>
+      </c>
+      <c r="E32" s="17">
         <v>2</v>
       </c>
     </row>
@@ -1836,10 +1836,10 @@
       <c r="C33" s="5">
         <v>2</v>
       </c>
-      <c r="D33" s="23">
-        <v>1</v>
-      </c>
-      <c r="E33" s="21">
+      <c r="D33" s="22">
+        <v>1</v>
+      </c>
+      <c r="E33" s="20">
         <v>5</v>
       </c>
     </row>
@@ -1847,7 +1847,7 @@
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="19">
+      <c r="D34" s="18">
         <v>2</v>
       </c>
     </row>
@@ -1855,7 +1855,7 @@
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="19">
+      <c r="D35" s="18">
         <v>3</v>
       </c>
     </row>
@@ -1863,7 +1863,7 @@
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="19">
+      <c r="D36" s="18">
         <v>4</v>
       </c>
       <c r="E36">
@@ -1874,10 +1874,10 @@
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="10"/>
-      <c r="D37" s="22">
-        <v>5</v>
-      </c>
-      <c r="E37" s="18">
+      <c r="D37" s="21">
+        <v>5</v>
+      </c>
+      <c r="E37" s="17">
         <v>4</v>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       <c r="C38" s="5">
         <v>3</v>
       </c>
-      <c r="D38" s="23">
+      <c r="D38" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="19">
+      <c r="D39" s="18">
         <v>2</v>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="19">
+      <c r="D40" s="18">
         <v>3</v>
       </c>
     </row>
@@ -1911,7 +1911,7 @@
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="19">
+      <c r="D41" s="18">
         <v>4</v>
       </c>
     </row>
@@ -1919,10 +1919,10 @@
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="22">
-        <v>5</v>
-      </c>
-      <c r="E42" s="18"/>
+      <c r="D42" s="21">
+        <v>5</v>
+      </c>
+      <c r="E42" s="17"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
@@ -1930,10 +1930,10 @@
       <c r="C43" s="5">
         <v>4</v>
       </c>
-      <c r="D43" s="23">
-        <v>1</v>
-      </c>
-      <c r="E43" s="21">
+      <c r="D43" s="22">
+        <v>1</v>
+      </c>
+      <c r="E43" s="20">
         <v>8</v>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="19">
+      <c r="D44" s="18">
         <v>2</v>
       </c>
     </row>
@@ -1949,7 +1949,7 @@
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="19">
+      <c r="D45" s="18">
         <v>3</v>
       </c>
     </row>
@@ -1957,7 +1957,7 @@
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="5"/>
-      <c r="D46" s="19">
+      <c r="D46" s="18">
         <v>4</v>
       </c>
     </row>
@@ -1965,10 +1965,10 @@
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="10"/>
-      <c r="D47" s="22">
-        <v>5</v>
-      </c>
-      <c r="E47" s="18">
+      <c r="D47" s="21">
+        <v>5</v>
+      </c>
+      <c r="E47" s="17">
         <v>2</v>
       </c>
     </row>
@@ -1978,7 +1978,7 @@
       <c r="C48" s="5">
         <v>5</v>
       </c>
-      <c r="D48" s="23">
+      <c r="D48" s="22">
         <v>1</v>
       </c>
       <c r="E48">
@@ -1989,7 +1989,7 @@
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="5"/>
-      <c r="D49" s="19">
+      <c r="D49" s="18">
         <v>2</v>
       </c>
     </row>
@@ -1997,7 +1997,7 @@
       <c r="A50" s="4"/>
       <c r="B50" s="3"/>
       <c r="C50" s="5"/>
-      <c r="D50" s="19">
+      <c r="D50" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2005,7 +2005,7 @@
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="5"/>
-      <c r="D51" s="19">
+      <c r="D51" s="18">
         <v>4</v>
       </c>
       <c r="E51">
@@ -2016,10 +2016,10 @@
       <c r="A52" s="13"/>
       <c r="B52" s="11"/>
       <c r="C52" s="10"/>
-      <c r="D52" s="22">
-        <v>5</v>
-      </c>
-      <c r="E52" s="18"/>
+      <c r="D52" s="21">
+        <v>5</v>
+      </c>
+      <c r="E52" s="17"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
@@ -2031,7 +2031,7 @@
       <c r="C53" s="5">
         <v>1</v>
       </c>
-      <c r="D53" s="23">
+      <c r="D53" s="22">
         <v>1</v>
       </c>
     </row>
@@ -2039,7 +2039,7 @@
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="5"/>
-      <c r="D54" s="19">
+      <c r="D54" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="5"/>
-      <c r="D55" s="19">
+      <c r="D55" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2055,7 +2055,7 @@
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="5"/>
-      <c r="D56" s="19">
+      <c r="D56" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2063,10 +2063,10 @@
       <c r="A57" s="4"/>
       <c r="B57" s="3"/>
       <c r="C57" s="10"/>
-      <c r="D57" s="22">
-        <v>5</v>
-      </c>
-      <c r="E57" s="18"/>
+      <c r="D57" s="21">
+        <v>5</v>
+      </c>
+      <c r="E57" s="17"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
@@ -2074,7 +2074,7 @@
       <c r="C58" s="5">
         <v>2</v>
       </c>
-      <c r="D58" s="23">
+      <c r="D58" s="22">
         <v>1</v>
       </c>
     </row>
@@ -2082,7 +2082,7 @@
       <c r="A59" s="4"/>
       <c r="B59" s="3"/>
       <c r="C59" s="5"/>
-      <c r="D59" s="19">
+      <c r="D59" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2090,7 +2090,7 @@
       <c r="A60" s="4"/>
       <c r="B60" s="3"/>
       <c r="C60" s="5"/>
-      <c r="D60" s="19">
+      <c r="D60" s="18">
         <v>3</v>
       </c>
       <c r="E60">
@@ -2101,7 +2101,7 @@
       <c r="A61" s="4"/>
       <c r="B61" s="3"/>
       <c r="C61" s="5"/>
-      <c r="D61" s="19">
+      <c r="D61" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2109,10 +2109,10 @@
       <c r="A62" s="4"/>
       <c r="B62" s="3"/>
       <c r="C62" s="10"/>
-      <c r="D62" s="22">
-        <v>5</v>
-      </c>
-      <c r="E62" s="18">
+      <c r="D62" s="21">
+        <v>5</v>
+      </c>
+      <c r="E62" s="17">
         <v>4</v>
       </c>
     </row>
@@ -2122,7 +2122,7 @@
       <c r="C63" s="5">
         <v>3</v>
       </c>
-      <c r="D63" s="23">
+      <c r="D63" s="22">
         <v>1</v>
       </c>
     </row>
@@ -2130,7 +2130,7 @@
       <c r="A64" s="4"/>
       <c r="B64" s="3"/>
       <c r="C64" s="5"/>
-      <c r="D64" s="19">
+      <c r="D64" s="18">
         <v>2</v>
       </c>
       <c r="E64">
@@ -2141,7 +2141,7 @@
       <c r="A65" s="4"/>
       <c r="B65" s="3"/>
       <c r="C65" s="5"/>
-      <c r="D65" s="19">
+      <c r="D65" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2149,7 +2149,7 @@
       <c r="A66" s="4"/>
       <c r="B66" s="3"/>
       <c r="C66" s="5"/>
-      <c r="D66" s="19">
+      <c r="D66" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2157,10 +2157,10 @@
       <c r="A67" s="4"/>
       <c r="B67" s="3"/>
       <c r="C67" s="10"/>
-      <c r="D67" s="22">
-        <v>5</v>
-      </c>
-      <c r="E67" s="18">
+      <c r="D67" s="21">
+        <v>5</v>
+      </c>
+      <c r="E67" s="17">
         <v>5</v>
       </c>
     </row>
@@ -2170,7 +2170,7 @@
       <c r="C68" s="5">
         <v>4</v>
       </c>
-      <c r="D68" s="23">
+      <c r="D68" s="22">
         <v>1</v>
       </c>
     </row>
@@ -2178,7 +2178,7 @@
       <c r="A69" s="4"/>
       <c r="B69" s="3"/>
       <c r="C69" s="5"/>
-      <c r="D69" s="19">
+      <c r="D69" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2186,7 +2186,7 @@
       <c r="A70" s="4"/>
       <c r="B70" s="3"/>
       <c r="C70" s="5"/>
-      <c r="D70" s="19">
+      <c r="D70" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2194,7 +2194,7 @@
       <c r="A71" s="4"/>
       <c r="B71" s="3"/>
       <c r="C71" s="5"/>
-      <c r="D71" s="19">
+      <c r="D71" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2202,10 +2202,10 @@
       <c r="A72" s="4"/>
       <c r="B72" s="3"/>
       <c r="C72" s="10"/>
-      <c r="D72" s="22">
-        <v>5</v>
-      </c>
-      <c r="E72" s="18"/>
+      <c r="D72" s="21">
+        <v>5</v>
+      </c>
+      <c r="E72" s="17"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
@@ -2213,7 +2213,7 @@
       <c r="C73" s="5">
         <v>5</v>
       </c>
-      <c r="D73" s="23">
+      <c r="D73" s="22">
         <v>1</v>
       </c>
     </row>
@@ -2221,7 +2221,7 @@
       <c r="A74" s="4"/>
       <c r="B74" s="3"/>
       <c r="C74" s="5"/>
-      <c r="D74" s="19">
+      <c r="D74" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       <c r="A75" s="4"/>
       <c r="B75" s="3"/>
       <c r="C75" s="5"/>
-      <c r="D75" s="19">
+      <c r="D75" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       <c r="A76" s="4"/>
       <c r="B76" s="3"/>
       <c r="C76" s="5"/>
-      <c r="D76" s="19">
+      <c r="D76" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2245,10 +2245,10 @@
       <c r="A77" s="4"/>
       <c r="B77" s="11"/>
       <c r="C77" s="10"/>
-      <c r="D77" s="22">
-        <v>5</v>
-      </c>
-      <c r="E77" s="18"/>
+      <c r="D77" s="21">
+        <v>5</v>
+      </c>
+      <c r="E77" s="17"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
@@ -2258,7 +2258,7 @@
       <c r="C78" s="5">
         <v>1</v>
       </c>
-      <c r="D78" s="23">
+      <c r="D78" s="22">
         <v>1</v>
       </c>
     </row>
@@ -2266,7 +2266,7 @@
       <c r="A79" s="4"/>
       <c r="B79" s="3"/>
       <c r="C79" s="5"/>
-      <c r="D79" s="19">
+      <c r="D79" s="18">
         <v>2</v>
       </c>
       <c r="E79">
@@ -2277,7 +2277,7 @@
       <c r="A80" s="4"/>
       <c r="B80" s="3"/>
       <c r="C80" s="5"/>
-      <c r="D80" s="19">
+      <c r="D80" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2285,7 +2285,7 @@
       <c r="A81" s="4"/>
       <c r="B81" s="3"/>
       <c r="C81" s="5"/>
-      <c r="D81" s="19">
+      <c r="D81" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2293,10 +2293,10 @@
       <c r="A82" s="4"/>
       <c r="B82" s="3"/>
       <c r="C82" s="10"/>
-      <c r="D82" s="22">
-        <v>5</v>
-      </c>
-      <c r="E82" s="18">
+      <c r="D82" s="21">
+        <v>5</v>
+      </c>
+      <c r="E82" s="17">
         <v>6</v>
       </c>
     </row>
@@ -2306,7 +2306,7 @@
       <c r="C83" s="5">
         <v>2</v>
       </c>
-      <c r="D83" s="23">
+      <c r="D83" s="22">
         <v>1</v>
       </c>
       <c r="E83">
@@ -2317,7 +2317,7 @@
       <c r="A84" s="4"/>
       <c r="B84" s="3"/>
       <c r="C84" s="5"/>
-      <c r="D84" s="19">
+      <c r="D84" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2325,7 +2325,7 @@
       <c r="A85" s="4"/>
       <c r="B85" s="3"/>
       <c r="C85" s="5"/>
-      <c r="D85" s="19">
+      <c r="D85" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2333,7 +2333,7 @@
       <c r="A86" s="4"/>
       <c r="B86" s="3"/>
       <c r="C86" s="5"/>
-      <c r="D86" s="19">
+      <c r="D86" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2341,10 +2341,10 @@
       <c r="A87" s="4"/>
       <c r="B87" s="3"/>
       <c r="C87" s="10"/>
-      <c r="D87" s="22">
-        <v>5</v>
-      </c>
-      <c r="E87" s="18">
+      <c r="D87" s="21">
+        <v>5</v>
+      </c>
+      <c r="E87" s="17">
         <v>2</v>
       </c>
     </row>
@@ -2354,7 +2354,7 @@
       <c r="C88" s="5">
         <v>3</v>
       </c>
-      <c r="D88" s="23">
+      <c r="D88" s="22">
         <v>1</v>
       </c>
     </row>
@@ -2362,7 +2362,7 @@
       <c r="A89" s="4"/>
       <c r="B89" s="3"/>
       <c r="C89" s="5"/>
-      <c r="D89" s="19">
+      <c r="D89" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2370,7 +2370,7 @@
       <c r="A90" s="4"/>
       <c r="B90" s="3"/>
       <c r="C90" s="5"/>
-      <c r="D90" s="19">
+      <c r="D90" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2378,7 +2378,7 @@
       <c r="A91" s="4"/>
       <c r="B91" s="3"/>
       <c r="C91" s="5"/>
-      <c r="D91" s="19">
+      <c r="D91" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2386,10 +2386,10 @@
       <c r="A92" s="4"/>
       <c r="B92" s="3"/>
       <c r="C92" s="10"/>
-      <c r="D92" s="22">
-        <v>5</v>
-      </c>
-      <c r="E92" s="18"/>
+      <c r="D92" s="21">
+        <v>5</v>
+      </c>
+      <c r="E92" s="17"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
@@ -2397,7 +2397,7 @@
       <c r="C93" s="5">
         <v>4</v>
       </c>
-      <c r="D93" s="23">
+      <c r="D93" s="22">
         <v>1</v>
       </c>
     </row>
@@ -2405,7 +2405,7 @@
       <c r="A94" s="4"/>
       <c r="B94" s="3"/>
       <c r="C94" s="5"/>
-      <c r="D94" s="19">
+      <c r="D94" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2413,7 +2413,7 @@
       <c r="A95" s="4"/>
       <c r="B95" s="3"/>
       <c r="C95" s="5"/>
-      <c r="D95" s="19">
+      <c r="D95" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2421,7 +2421,7 @@
       <c r="A96" s="4"/>
       <c r="B96" s="3"/>
       <c r="C96" s="5"/>
-      <c r="D96" s="19">
+      <c r="D96" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2429,10 +2429,10 @@
       <c r="A97" s="4"/>
       <c r="B97" s="3"/>
       <c r="C97" s="10"/>
-      <c r="D97" s="22">
-        <v>5</v>
-      </c>
-      <c r="E97" s="18"/>
+      <c r="D97" s="21">
+        <v>5</v>
+      </c>
+      <c r="E97" s="17"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
@@ -2440,7 +2440,7 @@
       <c r="C98" s="5">
         <v>5</v>
       </c>
-      <c r="D98" s="23">
+      <c r="D98" s="22">
         <v>1</v>
       </c>
       <c r="E98">
@@ -2451,7 +2451,7 @@
       <c r="A99" s="4"/>
       <c r="B99" s="3"/>
       <c r="C99" s="5"/>
-      <c r="D99" s="19">
+      <c r="D99" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2459,7 +2459,7 @@
       <c r="A100" s="4"/>
       <c r="B100" s="3"/>
       <c r="C100" s="5"/>
-      <c r="D100" s="19">
+      <c r="D100" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2467,7 +2467,7 @@
       <c r="A101" s="4"/>
       <c r="B101" s="3"/>
       <c r="C101" s="5"/>
-      <c r="D101" s="19">
+      <c r="D101" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2475,10 +2475,10 @@
       <c r="A102" s="13"/>
       <c r="B102" s="11"/>
       <c r="C102" s="10"/>
-      <c r="D102" s="22">
-        <v>5</v>
-      </c>
-      <c r="E102" s="18"/>
+      <c r="D102" s="21">
+        <v>5</v>
+      </c>
+      <c r="E102" s="17"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
@@ -2490,7 +2490,7 @@
       <c r="C103" s="5">
         <v>1</v>
       </c>
-      <c r="D103" s="23">
+      <c r="D103" s="22">
         <v>1</v>
       </c>
     </row>
@@ -2498,7 +2498,7 @@
       <c r="A104" s="4"/>
       <c r="B104" s="3"/>
       <c r="C104" s="5"/>
-      <c r="D104" s="19">
+      <c r="D104" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2506,7 +2506,7 @@
       <c r="A105" s="4"/>
       <c r="B105" s="3"/>
       <c r="C105" s="5"/>
-      <c r="D105" s="19">
+      <c r="D105" s="18">
         <v>3</v>
       </c>
       <c r="E105">
@@ -2517,7 +2517,7 @@
       <c r="A106" s="4"/>
       <c r="B106" s="3"/>
       <c r="C106" s="5"/>
-      <c r="D106" s="19">
+      <c r="D106" s="18">
         <v>4</v>
       </c>
       <c r="E106">
@@ -2528,10 +2528,10 @@
       <c r="A107" s="4"/>
       <c r="B107" s="3"/>
       <c r="C107" s="10"/>
-      <c r="D107" s="22">
-        <v>5</v>
-      </c>
-      <c r="E107" s="18">
+      <c r="D107" s="21">
+        <v>5</v>
+      </c>
+      <c r="E107" s="17">
         <v>9</v>
       </c>
     </row>
@@ -2541,7 +2541,7 @@
       <c r="C108" s="5">
         <v>2</v>
       </c>
-      <c r="D108" s="23">
+      <c r="D108" s="22">
         <v>1</v>
       </c>
     </row>
@@ -2549,7 +2549,7 @@
       <c r="A109" s="4"/>
       <c r="B109" s="3"/>
       <c r="C109" s="5"/>
-      <c r="D109" s="19">
+      <c r="D109" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2557,7 +2557,7 @@
       <c r="A110" s="4"/>
       <c r="B110" s="3"/>
       <c r="C110" s="5"/>
-      <c r="D110" s="19">
+      <c r="D110" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2565,7 +2565,7 @@
       <c r="A111" s="4"/>
       <c r="B111" s="3"/>
       <c r="C111" s="5"/>
-      <c r="D111" s="19">
+      <c r="D111" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2573,10 +2573,10 @@
       <c r="A112" s="4"/>
       <c r="B112" s="3"/>
       <c r="C112" s="10"/>
-      <c r="D112" s="22">
-        <v>5</v>
-      </c>
-      <c r="E112" s="18"/>
+      <c r="D112" s="21">
+        <v>5</v>
+      </c>
+      <c r="E112" s="17"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
@@ -2584,7 +2584,7 @@
       <c r="C113" s="5">
         <v>3</v>
       </c>
-      <c r="D113" s="23">
+      <c r="D113" s="22">
         <v>1</v>
       </c>
       <c r="E113">
@@ -2595,7 +2595,7 @@
       <c r="A114" s="4"/>
       <c r="B114" s="3"/>
       <c r="C114" s="5"/>
-      <c r="D114" s="19">
+      <c r="D114" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2603,7 +2603,7 @@
       <c r="A115" s="4"/>
       <c r="B115" s="3"/>
       <c r="C115" s="5"/>
-      <c r="D115" s="19">
+      <c r="D115" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2611,7 +2611,7 @@
       <c r="A116" s="4"/>
       <c r="B116" s="3"/>
       <c r="C116" s="5"/>
-      <c r="D116" s="19">
+      <c r="D116" s="18">
         <v>4</v>
       </c>
       <c r="E116">
@@ -2622,10 +2622,10 @@
       <c r="A117" s="4"/>
       <c r="B117" s="3"/>
       <c r="C117" s="10"/>
-      <c r="D117" s="22">
-        <v>5</v>
-      </c>
-      <c r="E117" s="18">
+      <c r="D117" s="21">
+        <v>5</v>
+      </c>
+      <c r="E117" s="17">
         <v>8</v>
       </c>
     </row>
@@ -2635,10 +2635,10 @@
       <c r="C118" s="5">
         <v>4</v>
       </c>
-      <c r="D118" s="23">
-        <v>1</v>
-      </c>
-      <c r="E118" s="21">
+      <c r="D118" s="22">
+        <v>1</v>
+      </c>
+      <c r="E118" s="20">
         <v>5</v>
       </c>
     </row>
@@ -2646,7 +2646,7 @@
       <c r="A119" s="4"/>
       <c r="B119" s="3"/>
       <c r="C119" s="5"/>
-      <c r="D119" s="19">
+      <c r="D119" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       <c r="A120" s="4"/>
       <c r="B120" s="3"/>
       <c r="C120" s="5"/>
-      <c r="D120" s="19">
+      <c r="D120" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2662,7 +2662,7 @@
       <c r="A121" s="4"/>
       <c r="B121" s="3"/>
       <c r="C121" s="5"/>
-      <c r="D121" s="19">
+      <c r="D121" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2670,10 +2670,10 @@
       <c r="A122" s="4"/>
       <c r="B122" s="3"/>
       <c r="C122" s="10"/>
-      <c r="D122" s="22">
-        <v>5</v>
-      </c>
-      <c r="E122" s="18">
+      <c r="D122" s="21">
+        <v>5</v>
+      </c>
+      <c r="E122" s="17">
         <v>2</v>
       </c>
     </row>
@@ -2683,7 +2683,7 @@
       <c r="C123" s="5">
         <v>5</v>
       </c>
-      <c r="D123" s="23">
+      <c r="D123" s="22">
         <v>1</v>
       </c>
       <c r="E123">
@@ -2694,7 +2694,7 @@
       <c r="A124" s="4"/>
       <c r="B124" s="3"/>
       <c r="C124" s="5"/>
-      <c r="D124" s="19">
+      <c r="D124" s="18">
         <v>2</v>
       </c>
     </row>
@@ -2702,7 +2702,7 @@
       <c r="A125" s="4"/>
       <c r="B125" s="3"/>
       <c r="C125" s="5"/>
-      <c r="D125" s="19">
+      <c r="D125" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2710,7 +2710,7 @@
       <c r="A126" s="4"/>
       <c r="B126" s="3"/>
       <c r="C126" s="5"/>
-      <c r="D126" s="19">
+      <c r="D126" s="18">
         <v>4</v>
       </c>
       <c r="E126">
@@ -2721,10 +2721,10 @@
       <c r="A127" s="13"/>
       <c r="B127" s="11"/>
       <c r="C127" s="10"/>
-      <c r="D127" s="22">
-        <v>5</v>
-      </c>
-      <c r="E127" s="18"/>
+      <c r="D127" s="21">
+        <v>5</v>
+      </c>
+      <c r="E127" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>